<commit_message>
Changed some test Cases
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
+++ b/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB6D943-FA0E-44CB-88BF-5AC6EEADDEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1DE1E4-C54A-4916-9F12-7A04BFD5554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{EB3F234C-04B7-4BC7-BB8F-A6184960D830}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Swim</t>
   </si>
   <si>
-    <t>Case Gaming</t>
-  </si>
-  <si>
     <t>Eu4</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Math</t>
+  </si>
+  <si>
+    <t>Deleted --- Case Gaming --- As we do not want to add this complexity</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -268,6 +268,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -275,15 +301,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -292,8 +317,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -589,6 +621,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -652,13 +691,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -771,8 +803,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}" name="Table39248101416" displayName="Table39248101416" ref="I30:J33" totalsRowShown="0">
-  <autoFilter ref="I30:J33" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}" name="Table39248101416" displayName="Table39248101416" ref="I24:J27" totalsRowShown="0">
+  <autoFilter ref="I24:J27" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4305C923-49DE-4C39-AB1E-8B401D39BA53}" name="Id" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{32755C06-5520-470A-B3AC-DB7AB1EB6659}" name="Name" dataDxfId="3"/>
@@ -782,8 +814,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}" name="Table2279131517" displayName="Table2279131517" ref="A37:G40" totalsRowShown="0" tableBorderDxfId="2" dataCellStyle="Good">
-  <autoFilter ref="A37:G40" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}" name="Table2279131517" displayName="Table2279131517" ref="A31:G34" totalsRowShown="0" tableBorderDxfId="2" dataCellStyle="Good">
+  <autoFilter ref="A31:G34" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{181FE9E7-3517-492D-A341-0471232A8352}" name="id" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{E0400840-62BA-44D2-807B-44AEA1F94E38}" name="StartTime" dataCellStyle="Good"/>
@@ -798,8 +830,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}" name="Table3924810141618" displayName="Table3924810141618" ref="I37:J40" totalsRowShown="0">
-  <autoFilter ref="I37:J40" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}" name="Table3924810141618" displayName="Table3924810141618" ref="I31:J34" totalsRowShown="0">
+  <autoFilter ref="I31:J34" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5989481F-75C2-4FF7-A14C-DE3759D908FC}" name="Id" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{65162EB8-1FD5-4B79-9448-52C7A5722C80}" name="Name" dataDxfId="0"/>
@@ -820,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{571964D9-2C3D-4516-BEBC-D5FBA6A6AAF9}" name="Table2279" displayName="Table2279" ref="A16:G19" totalsRowShown="0" tableBorderDxfId="14" dataCellStyle="Good">
-  <autoFilter ref="A16:G19" xr:uid="{571964D9-2C3D-4516-BEBC-D5FBA6A6AAF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{571964D9-2C3D-4516-BEBC-D5FBA6A6AAF9}" name="Table2279" displayName="Table2279" ref="A17:G20" totalsRowShown="0" tableBorderDxfId="14" dataCellStyle="Good">
+  <autoFilter ref="A17:G20" xr:uid="{571964D9-2C3D-4516-BEBC-D5FBA6A6AAF9}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9FB3BBD5-32F6-46EB-B455-7989F1AF448A}" name="id" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{7206F9C7-A09B-40A9-8D6E-E811CC0AAEE4}" name="StartTime" dataCellStyle="Good"/>
@@ -836,19 +868,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}" name="Table3924810" displayName="Table3924810" ref="I16:J19" totalsRowShown="0">
-  <autoFilter ref="I16:J19" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}" name="Table3924810" displayName="Table3924810" ref="I17:J20" totalsRowShown="0">
+  <autoFilter ref="I17:J20" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B857CB42-C590-4D59-8E07-E998AD47E171}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B5A559BD-D07F-4692-9170-B2E9A279141E}" name="Name" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B857CB42-C590-4D59-8E07-E998AD47E171}" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{B5A559BD-D07F-4692-9170-B2E9A279141E}" name="Name" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}" name="Table2211" displayName="Table2211" ref="A9:G12" totalsRowShown="0" tableBorderDxfId="13" dataCellStyle="Normal">
-  <autoFilter ref="A9:G12" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}" name="Table2211" displayName="Table2211" ref="A9:G13" totalsRowShown="0" tableBorderDxfId="11" dataCellStyle="Normal">
+  <autoFilter ref="A9:G13" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{09AE5FB9-C481-4F65-B7CE-417586905753}" name="id" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{3DC06B6F-3073-4529-ABFA-C46FD18389BE}" name="StartTime" dataCellStyle="Normal"/>
@@ -866,16 +898,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}" name="Table392412" displayName="Table392412" ref="I9:J11" totalsRowShown="0">
   <autoFilter ref="I9:J11" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{61910470-66DD-4232-8FAB-05D2FE5EC212}" name="Id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{7D6BEDF0-DD10-4C10-AA1B-876C52DE68B4}" name="Name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{61910470-66DD-4232-8FAB-05D2FE5EC212}" name="Id" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{7D6BEDF0-DD10-4C10-AA1B-876C52DE68B4}" name="Name" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}" name="Table227913" displayName="Table227913" ref="A23:G26" totalsRowShown="0" tableBorderDxfId="8" dataCellStyle="Good">
-  <autoFilter ref="A23:G26" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}" name="Table227913" displayName="Table227913" ref="M24:S27" totalsRowShown="0" tableBorderDxfId="8" dataCellStyle="Good">
+  <autoFilter ref="M24:S27" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E7C261B4-51F2-4A2A-A840-2D4814163034}" name="id" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{A1DCC69B-4577-478C-8D69-8B1ADA17C2D0}" name="StartTime" dataCellStyle="Good"/>
@@ -890,8 +922,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}" name="Table392481014" displayName="Table392481014" ref="I23:J25" totalsRowShown="0">
-  <autoFilter ref="I23:J25" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}" name="Table392481014" displayName="Table392481014" ref="U24:V26" totalsRowShown="0">
+  <autoFilter ref="U24:V26" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A7ECA230-DF09-4783-A5DE-31644D7391A1}" name="Id" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{8CA5AB6B-4E95-4E9B-A6B6-105671CC9D8A}" name="Name" dataDxfId="6"/>
@@ -901,8 +933,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}" name="Table22791315" displayName="Table22791315" ref="A30:G33" totalsRowShown="0" tableBorderDxfId="5" dataCellStyle="Good">
-  <autoFilter ref="A30:G33" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}" name="Table22791315" displayName="Table22791315" ref="A24:G27" totalsRowShown="0" tableBorderDxfId="5" dataCellStyle="Good">
+  <autoFilter ref="A24:G27" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6EFF49D4-4807-4900-9DDC-A648BDD1F242}" name="id" dataCellStyle="Good"/>
     <tableColumn id="2" xr3:uid="{06A9AFD1-2BFB-489B-BCD9-CC290EE06AFD}" name="StartTime" dataCellStyle="Good"/>
@@ -1213,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D53D22-FC72-43AC-BF1E-CBD4C9E417DE}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,33 +1257,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="I2" s="5" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1315,38 +1347,38 @@
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="I8" s="5" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="I8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1378,22 +1410,23 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="12">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="12">
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="D10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
         <v>2</v>
       </c>
       <c r="I10" s="1">
@@ -1404,286 +1437,333 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="12">
         <v>2</v>
       </c>
-      <c r="B11" s="10">
-        <v>14</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="b">
+      <c r="B11" s="12">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="12">
         <v>2</v>
       </c>
       <c r="I11">
         <v>4</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="12">
+        <v>14</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>14</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="b">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="5" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="I16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>2</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>3</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>14</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>8</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1">
-        <v>5</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
         <v>14</v>
       </c>
-      <c r="C18">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
+      <c r="F18" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="G18">
         <v>3</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="I19">
         <v>6</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>10</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C20" s="3">
         <v>14</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="b">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <v>3</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I20" s="4">
         <v>7</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J20" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="M22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="I22" s="5" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="I23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="J23" s="9"/>
+      <c r="M23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="U23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V23" s="11"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>0</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>2</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>3</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>14</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>8</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24">
+      <c r="M24" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" t="s">
+        <v>19</v>
+      </c>
+      <c r="O24" t="s">
+        <v>18</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R24" t="s">
+        <v>3</v>
+      </c>
+      <c r="S24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="U24" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
       <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
         <v>14</v>
       </c>
-      <c r="C25">
-        <v>16</v>
-      </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" s="3" t="b">
         <v>1</v>
@@ -1691,333 +1771,295 @@
       <c r="G25">
         <v>4</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
+        <v>8</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="O25">
+        <v>14</v>
+      </c>
+      <c r="P25" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="U25" s="1">
+        <v>8</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="I26">
         <v>9</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="J26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26">
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <v>14</v>
+      </c>
+      <c r="O26">
+        <v>16</v>
+      </c>
+      <c r="P26" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>4</v>
+      </c>
+      <c r="U26">
+        <v>9</v>
+      </c>
+      <c r="V26" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B27" s="3">
         <v>10</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C27" s="3">
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4</v>
+      </c>
+      <c r="I27" s="4">
+        <v>10</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="3">
+        <v>10</v>
+      </c>
+      <c r="O27" s="3">
         <v>16</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="b">
+      <c r="P27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G26" s="3">
+      <c r="S27" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="I29" s="5" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="I30" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>2</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>3</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>14</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>8</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31">
-        <v>14</v>
-      </c>
-      <c r="D31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="I31" s="1">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>
       <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
         <v>14</v>
       </c>
-      <c r="C32">
-        <v>16</v>
-      </c>
       <c r="D32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="F32" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="G32">
         <v>4</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>11</v>
       </c>
-      <c r="J32" s="9" t="s">
-        <v>30</v>
+      <c r="J32" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="I33">
         <v>12</v>
       </c>
-      <c r="B33" s="3">
+      <c r="J33" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3">
         <v>10</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C34" s="3">
         <v>14</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3" t="b">
+      <c r="D34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G34" s="3">
         <v>4</v>
       </c>
-      <c r="I33" s="8">
-        <v>12</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="I36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>9</v>
-      </c>
-      <c r="B38">
-        <v>10</v>
-      </c>
-      <c r="C38">
-        <v>14</v>
-      </c>
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="I38" s="1">
+      <c r="I34" s="4">
         <v>13</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39">
-        <v>14</v>
-      </c>
-      <c r="C39">
-        <v>16</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="J34" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>4</v>
-      </c>
-      <c r="I39">
-        <v>14</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="3">
-        <v>10</v>
-      </c>
-      <c r="C40" s="3">
-        <v>14</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G40" s="3">
-        <v>4</v>
-      </c>
-      <c r="I40" s="8">
-        <v>15</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A14:J14"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="A7:J7"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="M23:S23"/>
+    <mergeCell ref="M22:V22"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="I23:J23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Test cases to database
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
+++ b/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1DE1E4-C54A-4916-9F12-7A04BFD5554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ABE62-954C-48DD-9FF7-3700F9E39B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{EB3F234C-04B7-4BC7-BB8F-A6184960D830}"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3F234C-04B7-4BC7-BB8F-A6184960D830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -301,7 +301,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -327,6 +327,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -402,13 +404,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -691,6 +686,13 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -806,15 +808,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}" name="Table39248101416" displayName="Table39248101416" ref="I24:J27" totalsRowShown="0">
   <autoFilter ref="I24:J27" xr:uid="{04563E60-CC9B-4B95-BCAE-2BB456B2EDDE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4305C923-49DE-4C39-AB1E-8B401D39BA53}" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{32755C06-5520-470A-B3AC-DB7AB1EB6659}" name="Name" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{4305C923-49DE-4C39-AB1E-8B401D39BA53}" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{32755C06-5520-470A-B3AC-DB7AB1EB6659}" name="Name" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}" name="Table2279131517" displayName="Table2279131517" ref="A31:G34" totalsRowShown="0" tableBorderDxfId="2" dataCellStyle="Good">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}" name="Table2279131517" displayName="Table2279131517" ref="A31:G34" totalsRowShown="0" tableBorderDxfId="4" dataCellStyle="Good">
   <autoFilter ref="A31:G34" xr:uid="{F8B421AE-AB08-4494-AB74-0AE3B4150AD0}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{181FE9E7-3517-492D-A341-0471232A8352}" name="id" dataCellStyle="Good"/>
@@ -833,8 +835,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}" name="Table3924810141618" displayName="Table3924810141618" ref="I31:J34" totalsRowShown="0">
   <autoFilter ref="I31:J34" xr:uid="{4A35B966-564E-488E-9203-5BA90092D0A5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5989481F-75C2-4FF7-A14C-DE3759D908FC}" name="Id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{65162EB8-1FD5-4B79-9448-52C7A5722C80}" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5989481F-75C2-4FF7-A14C-DE3759D908FC}" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{65162EB8-1FD5-4B79-9448-52C7A5722C80}" name="Name" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,15 +873,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}" name="Table3924810" displayName="Table3924810" ref="I17:J20" totalsRowShown="0">
   <autoFilter ref="I17:J20" xr:uid="{A06CFC53-7BAD-4213-8367-7C7EC7529C78}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B857CB42-C590-4D59-8E07-E998AD47E171}" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{B5A559BD-D07F-4692-9170-B2E9A279141E}" name="Name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{B857CB42-C590-4D59-8E07-E998AD47E171}" name="Id" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B5A559BD-D07F-4692-9170-B2E9A279141E}" name="Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}" name="Table2211" displayName="Table2211" ref="A9:G13" totalsRowShown="0" tableBorderDxfId="11" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}" name="Table2211" displayName="Table2211" ref="A9:G13" totalsRowShown="0" tableBorderDxfId="13" dataCellStyle="Normal">
   <autoFilter ref="A9:G13" xr:uid="{E4E55830-EA0D-43E9-AD32-32E1F3866EFA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{09AE5FB9-C481-4F65-B7CE-417586905753}" name="id" dataCellStyle="Normal"/>
@@ -895,18 +897,18 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}" name="Table392412" displayName="Table392412" ref="I9:J11" totalsRowShown="0">
-  <autoFilter ref="I9:J11" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}" name="Table392412" displayName="Table392412" ref="I9:J12" totalsRowShown="0">
+  <autoFilter ref="I9:J12" xr:uid="{08AFAE42-3C76-4A25-A754-CB563106179B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{61910470-66DD-4232-8FAB-05D2FE5EC212}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{7D6BEDF0-DD10-4C10-AA1B-876C52DE68B4}" name="Name" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{61910470-66DD-4232-8FAB-05D2FE5EC212}" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7D6BEDF0-DD10-4C10-AA1B-876C52DE68B4}" name="Name" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}" name="Table227913" displayName="Table227913" ref="M24:S27" totalsRowShown="0" tableBorderDxfId="8" dataCellStyle="Good">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}" name="Table227913" displayName="Table227913" ref="M24:S27" totalsRowShown="0" tableBorderDxfId="10" dataCellStyle="Good">
   <autoFilter ref="M24:S27" xr:uid="{C0A99AE3-8AD9-4DE2-9595-6083B4D0B364}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E7C261B4-51F2-4A2A-A840-2D4814163034}" name="id" dataCellStyle="Good"/>
@@ -925,15 +927,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}" name="Table392481014" displayName="Table392481014" ref="U24:V26" totalsRowShown="0">
   <autoFilter ref="U24:V26" xr:uid="{3550EB0B-3F73-4764-9AAE-26E64341C7E3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A7ECA230-DF09-4783-A5DE-31644D7391A1}" name="Id" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8CA5AB6B-4E95-4E9B-A6B6-105671CC9D8A}" name="Name" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A7ECA230-DF09-4783-A5DE-31644D7391A1}" name="Id" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8CA5AB6B-4E95-4E9B-A6B6-105671CC9D8A}" name="Name" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}" name="Table22791315" displayName="Table22791315" ref="A24:G27" totalsRowShown="0" tableBorderDxfId="5" dataCellStyle="Good">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}" name="Table22791315" displayName="Table22791315" ref="A24:G27" totalsRowShown="0" tableBorderDxfId="7" dataCellStyle="Good">
   <autoFilter ref="A24:G27" xr:uid="{AD63EB93-1E2F-48FB-95B0-F0B07164ACE4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6EFF49D4-4807-4900-9DDC-A648BDD1F242}" name="id" dataCellStyle="Good"/>
@@ -1248,7 +1250,7 @@
   <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,6 +1485,12 @@
       <c r="G12" s="12">
         <v>2</v>
       </c>
+      <c r="I12" s="13">
+        <v>5</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1583,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="I18" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>16</v>
@@ -1609,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="I19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>17</v>
@@ -1636,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>24</v>
@@ -1772,7 +1780,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>28</v>
@@ -1825,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="I26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>29</v>
@@ -1876,7 +1884,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>30</v>
@@ -1976,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I32" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>32</v>
@@ -2002,10 +2010,10 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I33">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>33</v>
@@ -2031,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I34" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added extra case to RollBackService
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
+++ b/Documentation/Design Analysis/EntryAdderAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDAEAD4-6CC7-4A2E-90E2-A28030A502B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D96A9D2-64F3-416F-9E85-1FA0FEF08E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{EB3F234C-04B7-4BC7-BB8F-A6184960D830}"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{EB3F234C-04B7-4BC7-BB8F-A6184960D830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1141,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D53D22-FC72-43AC-BF1E-CBD4C9E417DE}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>